<commit_message>
Backend listo para despliegue
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Fecha</t>
   </si>
@@ -35,6 +35,30 @@
   </si>
   <si>
     <t>Autos</t>
+  </si>
+  <si>
+    <t>15/10/2025, 12:17:46 a. m.</t>
+  </si>
+  <si>
+    <t>Dania</t>
+  </si>
+  <si>
+    <t>Soto</t>
+  </si>
+  <si>
+    <t>Voleibol</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>Jutiapa</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Toyota</t>
   </si>
 </sst>
 </file>
@@ -411,11 +435,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="3" width="20" customWidth="1"/>
-    <col min="4" max="5" width="15" customWidth="1"/>
+    <col min="1" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
     <col min="8" max="8" width="30" customWidth="1"/>
@@ -447,8 +471,34 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>